<commit_message>
Retoques a las tablas, complejidad de los algoritmos (no se si esta bien)
</commit_message>
<xml_diff>
--- a/documentacion/Tablas de rendimiento comparativo.xlsx
+++ b/documentacion/Tablas de rendimiento comparativo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Recursiva</t>
   </si>
@@ -55,12 +55,49 @@
   <si>
     <t>tiempo (ms)</t>
   </si>
+  <si>
+    <t>OutOfMemory</t>
+  </si>
+  <si>
+    <r>
+      <t>Complejidad: O(n</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Complejidad: O(n*log(n))</t>
+  </si>
+  <si>
+    <t>Complejidad: O(n)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +108,23 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -164,19 +218,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -188,6 +284,32 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,6 +447,51 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$C$25:$C$40</c:f>
@@ -427,7 +594,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -435,11 +601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302108256"/>
-        <c:axId val="302107864"/>
+        <c:axId val="224873400"/>
+        <c:axId val="224870656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302108256"/>
+        <c:axId val="224873400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,12 +718,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302107864"/>
+        <c:crossAx val="224870656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302107864"/>
+        <c:axId val="224870656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +835,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302108256"/>
+        <c:crossAx val="224873400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -849,6 +1015,51 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$C$45:$C$60</c:f>
@@ -970,11 +1181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92387936"/>
-        <c:axId val="92388328"/>
+        <c:axId val="224875360"/>
+        <c:axId val="224869872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92387936"/>
+        <c:axId val="224875360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,12 +1298,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92388328"/>
+        <c:crossAx val="224869872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92388328"/>
+        <c:axId val="224869872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,7 +1415,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92387936"/>
+        <c:crossAx val="224875360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1384,12 +1595,57 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$65:$C$80</c:f>
+              <c:f>Hoja1!$C$65:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1437,16 +1693,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$65:$D$80</c:f>
+              <c:f>Hoja1!$D$65:$D$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1494,6 +1759,15 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>882</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1748</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,11 +1782,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="459182536"/>
-        <c:axId val="459184104"/>
+        <c:axId val="224869088"/>
+        <c:axId val="118435752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="459182536"/>
+        <c:axId val="224869088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1625,12 +1899,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459184104"/>
+        <c:crossAx val="118435752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="459184104"/>
+        <c:axId val="118435752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,7 +2016,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459182536"/>
+        <c:crossAx val="224869088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1895,7 +2169,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$83</c:f>
+              <c:f>Hoja1!$C$86</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1922,12 +2196,57 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$85:$C$100</c:f>
+              <c:f>Hoja1!$C$88:$C$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1975,16 +2294,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$85:$D$100</c:f>
+              <c:f>Hoja1!$D$88:$D$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2032,6 +2360,15 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2046,11 +2383,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121987024"/>
-        <c:axId val="121987416"/>
+        <c:axId val="147699888"/>
+        <c:axId val="312380408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121987024"/>
+        <c:axId val="147699888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,12 +2500,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121987416"/>
+        <c:crossAx val="312380408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121987416"/>
+        <c:axId val="312380408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2280,7 +2617,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121987024"/>
+        <c:crossAx val="147699888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2433,7 +2770,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$103</c:f>
+              <c:f>Hoja1!$C$110</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2460,12 +2797,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$105:$C$120</c:f>
+              <c:f>Hoja1!$C$112:$C$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2513,16 +2894,22 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$105:$D$120</c:f>
+              <c:f>Hoja1!$D$112:$D$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2570,6 +2957,12 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2584,11 +2977,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302842200"/>
-        <c:axId val="302847296"/>
+        <c:axId val="312380800"/>
+        <c:axId val="312381192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302842200"/>
+        <c:axId val="312380800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2701,12 +3094,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302847296"/>
+        <c:crossAx val="312381192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302847296"/>
+        <c:axId val="312381192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2818,7 +3211,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302842200"/>
+        <c:crossAx val="312380800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2971,7 +3364,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$123</c:f>
+              <c:f>Hoja1!$C$134</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2998,12 +3391,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$125:$C$140</c:f>
+              <c:f>Hoja1!$C$136:$C$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3051,16 +3488,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$125:$D$140</c:f>
+              <c:f>Hoja1!$D$136:$D$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3108,6 +3554,15 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3122,11 +3577,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302844552"/>
-        <c:axId val="302846904"/>
+        <c:axId val="312382368"/>
+        <c:axId val="312381584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302844552"/>
+        <c:axId val="312382368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3239,12 +3694,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302846904"/>
+        <c:crossAx val="312381584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302846904"/>
+        <c:axId val="312381584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3356,7 +3811,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302844552"/>
+        <c:crossAx val="312382368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3509,7 +3964,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$143</c:f>
+              <c:f>Hoja1!$C$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3536,12 +3991,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$145:$C$160</c:f>
+              <c:f>Hoja1!$C$166:$C$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3589,16 +4088,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$145:$D$160</c:f>
+              <c:f>Hoja1!$D$166:$D$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3646,6 +4154,15 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3660,11 +4177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198162568"/>
-        <c:axId val="198161784"/>
+        <c:axId val="312381976"/>
+        <c:axId val="312376488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198162568"/>
+        <c:axId val="312381976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,12 +4294,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198161784"/>
+        <c:crossAx val="312376488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198161784"/>
+        <c:axId val="312376488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3894,7 +4411,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198162568"/>
+        <c:crossAx val="312381976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4344,10 +4861,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$65:$C$80</c:f>
+              <c:f>Hoja1!$C$65:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4395,16 +4912,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$65:$D$80</c:f>
+              <c:f>Hoja1!$D$65:$D$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4452,6 +4978,15 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>882</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1748</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4463,7 +4998,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$83</c:f>
+              <c:f>Hoja1!$C$86</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4492,10 +5027,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$85:$C$100</c:f>
+              <c:f>Hoja1!$C$88:$C$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4543,16 +5078,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$85:$D$100</c:f>
+              <c:f>Hoja1!$D$88:$D$106</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4600,6 +5144,15 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4611,7 +5164,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$103</c:f>
+              <c:f>Hoja1!$C$110</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4640,10 +5193,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$105:$C$120</c:f>
+              <c:f>Hoja1!$C$112:$C$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4691,16 +5244,22 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$105:$D$120</c:f>
+              <c:f>Hoja1!$D$112:$D$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4749,153 +5308,11 @@
                 <c:pt idx="15">
                   <c:v>5</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$C$123</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Prog. Dinámica Mejorada</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="9525" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Hoja1!$C$125:$C$140</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>75000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Hoja1!$D$125:$D$140</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
+                <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4904,10 +5321,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$143</c:f>
+              <c:f>Hoja1!$C$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4938,10 +5355,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$145:$C$160</c:f>
+              <c:f>Hoja1!$C$166:$C$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4989,16 +5406,25 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$145:$D$160</c:f>
+              <c:f>Hoja1!$D$166:$D$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5046,6 +5472,181 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>246</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$134</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prog. Dinámica Mejorada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$136:$C$154</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$136:$D$154</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5060,11 +5661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302137808"/>
-        <c:axId val="302137416"/>
+        <c:axId val="312383544"/>
+        <c:axId val="312383936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302137808"/>
+        <c:axId val="312383544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5177,15 +5778,15 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302137416"/>
+        <c:crossAx val="312383936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302137416"/>
+        <c:axId val="312383936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
+          <c:max val="2000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5295,7 +5896,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302137808"/>
+        <c:crossAx val="312383544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9757,15 +10358,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9789,15 +10390,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>723901</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9821,15 +10422,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9853,15 +10454,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9885,15 +10486,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9917,15 +10518,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10244,10 +10845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D160"/>
+  <dimension ref="B1:J184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M167" sqref="M167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10260,7 +10861,7 @@
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="14.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
     <col min="11" max="12" width="11.42578125" style="1"/>
     <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
     <col min="14" max="15" width="11.42578125" style="1" customWidth="1"/>
@@ -10290,1014 +10891,1214 @@
     <row r="21" spans="3:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="3:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="3:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="8">
+      <c r="C25" s="6">
         <v>1</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>10</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <v>25</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>50</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <v>100</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="6">
+      <c r="C30" s="4">
         <v>250</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <v>500</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="6">
+      <c r="C32" s="4">
         <v>1000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="6">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="4">
         <v>2500</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="6">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="4">
         <v>5000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="6">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="4">
         <v>10000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="4">
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="6">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="4">
         <v>25000</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="6">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="4">
         <v>50000</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="6">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="4">
         <v>75000</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="6">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="4">
         <v>100000</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="6">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="4">
         <v>1000000</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="3:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="2" t="s">
+    <row r="41" spans="3:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="G41" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="3:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="4" t="s">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="8">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="6">
         <v>1</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="6">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="4">
         <v>10</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="6">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="4">
         <v>25</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="6">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="4">
         <v>50</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="6">
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="4">
         <v>100</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="6">
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="4">
         <v>250</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="6">
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="4">
         <v>500</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="6">
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="4">
         <v>1000</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="6">
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="4">
         <v>2500</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="6">
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="4">
         <v>5000</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="6">
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="4">
         <v>10000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="4">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="6">
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="4">
         <v>25000</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="5">
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="6">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="4">
         <v>50000</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="5">
         <v>1625</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="6">
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="4">
         <v>75000</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="5">
         <v>3630</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="6">
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C59" s="4">
         <v>100000</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="5">
         <v>6443</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="6">
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C60" s="4">
         <v>1000000</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="5">
         <v>649213</v>
       </c>
     </row>
-    <row r="62" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="2" t="s">
+    <row r="61" spans="3:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="G61" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="4" t="s">
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="8">
+      <c r="C65" s="6">
         <v>1</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="6">
+      <c r="C66" s="4">
         <v>10</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="6">
+      <c r="C67" s="4">
         <v>25</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="6">
+      <c r="C68" s="4">
         <v>50</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="6">
+      <c r="C69" s="4">
         <v>100</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="6">
+      <c r="C70" s="4">
         <v>250</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="6">
+      <c r="C71" s="4">
         <v>500</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="6">
+      <c r="C72" s="4">
         <v>1000</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="6">
+      <c r="C73" s="4">
         <v>2500</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="6">
+      <c r="C74" s="4">
         <v>5000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="6">
+      <c r="C75" s="4">
         <v>10000</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="6">
+      <c r="C76" s="4">
         <v>25000</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="6">
+      <c r="C77" s="4">
         <v>50000</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="6">
+      <c r="C78" s="4">
         <v>75000</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="5">
         <v>29</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="6">
+      <c r="C79" s="4">
         <v>100000</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D79" s="5">
         <v>38</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="6">
+      <c r="C80" s="4">
         <v>1000000</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="5">
         <v>344</v>
       </c>
     </row>
-    <row r="82" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="3:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C83" s="2" t="s">
+    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C81" s="4">
+        <v>2500000</v>
+      </c>
+      <c r="D81" s="4">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C82" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="D82" s="10">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="83" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="D83" s="4">
+        <v>3481</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+    </row>
+    <row r="85" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="3:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C84" s="4" t="s">
+      <c r="D86" s="8"/>
+    </row>
+    <row r="87" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D87" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="8">
+    <row r="88" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="6">
         <v>1</v>
-      </c>
-      <c r="D85" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="6">
-        <v>10</v>
-      </c>
-      <c r="D86" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="6">
-        <v>25</v>
-      </c>
-      <c r="D87" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="6">
-        <v>50</v>
       </c>
       <c r="D88" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="6">
+    <row r="89" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="4">
+        <v>10</v>
+      </c>
+      <c r="D89" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C90" s="4">
+        <v>25</v>
+      </c>
+      <c r="D90" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C91" s="4">
+        <v>50</v>
+      </c>
+      <c r="D91" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C92" s="4">
         <v>100</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D92" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="6">
+    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C93" s="4">
         <v>250</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D93" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="6">
+    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C94" s="4">
         <v>500</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D94" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="6">
+    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C95" s="4">
         <v>1000</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D95" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="6">
+    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C96" s="4">
         <v>2500</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D96" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="6">
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C97" s="4">
         <v>5000</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D97" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="6">
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C98" s="4">
         <v>10000</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D98" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C96" s="6">
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C99" s="4">
         <v>25000</v>
       </c>
-      <c r="D96" s="7">
+      <c r="D99" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="6">
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C100" s="4">
         <v>50000</v>
       </c>
-      <c r="D97" s="7">
+      <c r="D100" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C98" s="6">
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C101" s="4">
         <v>75000</v>
       </c>
-      <c r="D98" s="7">
+      <c r="D101" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="6">
+    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C102" s="4">
         <v>100000</v>
       </c>
-      <c r="D99" s="7">
+      <c r="D102" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C100" s="6">
+    <row r="103" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="4">
         <v>1000000</v>
       </c>
-      <c r="D100" s="7">
+      <c r="D103" s="5">
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="3:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C103" s="2" t="s">
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C104" s="9">
+        <v>5000000</v>
+      </c>
+      <c r="D104" s="4">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C105" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="D105" s="4">
+        <v>834</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="11"/>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C106" s="4">
+        <v>25000000</v>
+      </c>
+      <c r="D106" s="4">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="108" spans="3:10" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="3:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C110" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C104" s="4" t="s">
+      <c r="D110" s="8"/>
+    </row>
+    <row r="111" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C111" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="D111" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C105" s="8">
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C112" s="6">
         <v>1</v>
-      </c>
-      <c r="D105" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C106" s="6">
-        <v>10</v>
-      </c>
-      <c r="D106" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C107" s="6">
-        <v>25</v>
-      </c>
-      <c r="D107" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C108" s="6">
-        <v>50</v>
-      </c>
-      <c r="D108" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C109" s="6">
-        <v>100</v>
-      </c>
-      <c r="D109" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C110" s="6">
-        <v>250</v>
-      </c>
-      <c r="D110" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C111" s="6">
-        <v>500</v>
-      </c>
-      <c r="D111" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" s="6">
-        <v>1000</v>
       </c>
       <c r="D112" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C113" s="6">
+      <c r="C113" s="4">
+        <v>10</v>
+      </c>
+      <c r="D113" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="4">
+        <v>25</v>
+      </c>
+      <c r="D114" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="4">
+        <v>50</v>
+      </c>
+      <c r="D115" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="4">
+        <v>100</v>
+      </c>
+      <c r="D116" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="4">
+        <v>250</v>
+      </c>
+      <c r="D117" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="4">
+        <v>500</v>
+      </c>
+      <c r="D118" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D119" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" s="4">
         <v>2500</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D120" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C114" s="6">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="4">
         <v>5000</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D121" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="6">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="4">
         <v>10000</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D122" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C116" s="6">
+    <row r="123" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C123" s="4">
         <v>25000</v>
       </c>
-      <c r="D116" s="7">
+      <c r="D123" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C117" s="6">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="4">
         <v>50000</v>
       </c>
-      <c r="D117" s="7">
+      <c r="D124" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C118" s="6">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="4">
         <v>75000</v>
       </c>
-      <c r="D118" s="7">
+      <c r="D125" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C119" s="6">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="4">
         <v>100000</v>
       </c>
-      <c r="D119" s="7">
+      <c r="D126" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C120" s="6">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="4">
         <v>1000000</v>
       </c>
-      <c r="D120" s="7">
+      <c r="D127" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="3:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C123" s="2" t="s">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C128" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="D128" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C129" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="D129" s="4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="130" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C130" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G130" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
+      <c r="J130" s="16"/>
+    </row>
+    <row r="131" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C131" s="4">
+        <v>1000000000</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="3:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D123" s="3"/>
-    </row>
-    <row r="124" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C124" s="4" t="s">
+      <c r="D134" s="8"/>
+    </row>
+    <row r="135" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D135" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C125" s="8">
+    <row r="136" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C136" s="6">
         <v>1</v>
       </c>
-      <c r="D125" s="8">
+      <c r="D136" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C126" s="6">
+    <row r="137" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C137" s="4">
         <v>10</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D137" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C127" s="6">
+    <row r="138" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C138" s="4">
         <v>25</v>
       </c>
-      <c r="D127" s="6">
+      <c r="D138" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C128" s="6">
+    <row r="139" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C139" s="4">
         <v>50</v>
       </c>
-      <c r="D128" s="6">
+      <c r="D139" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C129" s="6">
+    <row r="140" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C140" s="4">
         <v>100</v>
       </c>
-      <c r="D129" s="6">
+      <c r="D140" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C130" s="6">
+    <row r="141" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C141" s="4">
         <v>250</v>
       </c>
-      <c r="D130" s="6">
+      <c r="D141" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C131" s="6">
+    <row r="142" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C142" s="4">
         <v>500</v>
       </c>
-      <c r="D131" s="6">
+      <c r="D142" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C132" s="6">
+    <row r="143" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C143" s="4">
         <v>1000</v>
       </c>
-      <c r="D132" s="6">
+      <c r="D143" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C133" s="6">
+    <row r="144" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C144" s="4">
         <v>2500</v>
       </c>
-      <c r="D133" s="6">
+      <c r="D144" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C134" s="6">
+    <row r="145" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C145" s="4">
         <v>5000</v>
       </c>
-      <c r="D134" s="6">
+      <c r="D145" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C135" s="6">
+    <row r="146" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C146" s="4">
         <v>10000</v>
       </c>
-      <c r="D135" s="6">
+      <c r="D146" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C136" s="6">
+    <row r="147" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C147" s="4">
         <v>25000</v>
       </c>
-      <c r="D136" s="7">
+      <c r="D147" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C137" s="6">
+    <row r="148" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C148" s="4">
         <v>50000</v>
       </c>
-      <c r="D137" s="7">
+      <c r="D148" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C138" s="6">
+    <row r="149" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C149" s="4">
         <v>75000</v>
       </c>
-      <c r="D138" s="7">
+      <c r="D149" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C139" s="6">
+    <row r="150" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C150" s="4">
         <v>100000</v>
       </c>
-      <c r="D139" s="7">
+      <c r="D150" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C140" s="6">
+    <row r="151" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C151" s="4">
         <v>1000000</v>
       </c>
-      <c r="D140" s="7">
+      <c r="D151" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="143" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C143" s="2" t="s">
+    <row r="152" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C152" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="D152" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="153" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C153" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="D153" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="154" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C154" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="D154" s="5">
+        <v>151</v>
+      </c>
+      <c r="G154" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H154" s="11"/>
+      <c r="I154" s="11"/>
+      <c r="J154" s="11"/>
+    </row>
+    <row r="155" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
+    </row>
+    <row r="156" spans="3:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
+    </row>
+    <row r="157" spans="3:10" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="3:10" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="159" spans="3:10" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="160" spans="3:10" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="161" spans="3:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="3:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="163" spans="3:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="164" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C164" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D143" s="3"/>
-    </row>
-    <row r="144" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C144" s="4" t="s">
+      <c r="D164" s="8"/>
+    </row>
+    <row r="165" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D144" s="5" t="s">
+      <c r="D165" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C145" s="8">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C166" s="6">
         <v>1</v>
       </c>
-      <c r="D145" s="8">
+      <c r="D166" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C146" s="6">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C167" s="4">
         <v>10</v>
       </c>
-      <c r="D146" s="6">
+      <c r="D167" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C147" s="6">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C168" s="4">
         <v>25</v>
       </c>
-      <c r="D147" s="6">
+      <c r="D168" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C148" s="6">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C169" s="4">
         <v>50</v>
       </c>
-      <c r="D148" s="6">
+      <c r="D169" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C149" s="6">
+    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C170" s="4">
         <v>100</v>
       </c>
-      <c r="D149" s="6">
+      <c r="D170" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C150" s="6">
+    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C171" s="4">
         <v>250</v>
       </c>
-      <c r="D150" s="6">
+      <c r="D171" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C151" s="6">
+    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C172" s="4">
         <v>500</v>
       </c>
-      <c r="D151" s="6">
+      <c r="D172" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C152" s="6">
+    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C173" s="4">
         <v>1000</v>
       </c>
-      <c r="D152" s="6">
+      <c r="D173" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C153" s="6">
+    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C174" s="4">
         <v>2500</v>
       </c>
-      <c r="D153" s="6">
+      <c r="D174" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C154" s="6">
+    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C175" s="4">
         <v>5000</v>
       </c>
-      <c r="D154" s="6">
+      <c r="D175" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C155" s="6">
+    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C176" s="4">
         <v>10000</v>
       </c>
-      <c r="D155" s="6">
+      <c r="D176" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C156" s="6">
+    <row r="177" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C177" s="4">
         <v>25000</v>
       </c>
-      <c r="D156" s="7">
+      <c r="D177" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C157" s="6">
+    <row r="178" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C178" s="4">
         <v>50000</v>
       </c>
-      <c r="D157" s="7">
+      <c r="D178" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C158" s="6">
+    <row r="179" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C179" s="4">
         <v>75000</v>
       </c>
-      <c r="D158" s="7">
+      <c r="D179" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C159" s="6">
+    <row r="180" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C180" s="4">
         <v>100000</v>
       </c>
-      <c r="D159" s="7">
+      <c r="D180" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C160" s="6">
+    <row r="181" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C181" s="4">
         <v>1000000</v>
       </c>
-      <c r="D160" s="7">
+      <c r="D181" s="5">
         <v>1</v>
       </c>
     </row>
+    <row r="182" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C182" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="D182" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="183" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C183" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="D183" s="4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="184" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C184" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="D184" s="5">
+        <v>246</v>
+      </c>
+      <c r="G184" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H184" s="11"/>
+      <c r="I184" s="11"/>
+      <c r="J184" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="G130:J130"/>
+    <mergeCell ref="G154:J154"/>
+    <mergeCell ref="G184:J184"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G61:J61"/>
+    <mergeCell ref="G83:J83"/>
+    <mergeCell ref="G105:J105"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C86:D86"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C110:D110"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C123:D123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>